<commit_message>
PS script for all in 02.TestData
</commit_message>
<xml_diff>
--- a/CI/TestSQL/03.TestConfigData/Participants/CreateGroupParticipants.xlsx
+++ b/CI/TestSQL/03.TestConfigData/Participants/CreateGroupParticipants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahHenney\Documents\GitSources\crds-angular\CI\TestSQL\03.TestConfigData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahHenney\Documents\GitSources\crds-angular\CI\TestSQL\03.TestConfigData\Participants\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t>_Last_Attendance</t>
   </si>
@@ -179,9 +179,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8747FACD-F75B-47C2-87CA-33CB79900CC9}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1015,7 +1016,22 @@
         <v>42125</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1">
+        <v>42309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>